<commit_message>
Login and signup system Finished
</commit_message>
<xml_diff>
--- a/assets/add_member_template.xlsx
+++ b/assets/add_member_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>region</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Nafih@gmail.com</t>
+  </si>
+  <si>
+    <t>coimbatore</t>
+  </si>
+  <si>
+    <t>ruralcoimbatore</t>
+  </si>
+  <si>
+    <t>ambition</t>
   </si>
 </sst>
 </file>
@@ -417,7 +426,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -454,11 +463,11 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -480,11 +489,11 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>

</xml_diff>